<commit_message>
modified:   Documents/presentation doc/Final Presentation/final-presentation.pptx
</commit_message>
<xml_diff>
--- a/Documents/weekly report/project plan.xlsx
+++ b/Documents/weekly report/project plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="20730" windowHeight="10020"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$T$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$T$40</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
   <si>
     <t>주제 선정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,27 +127,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Device Driver</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Device Driver</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USB/IP Porting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VHCI Driver</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Stub_driver.c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bind-driver.c</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -295,7 +279,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Odroid 터미널에서 실행</t>
+    <t>Bind-driver.c</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -742,7 +726,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -860,8 +844,74 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -890,77 +940,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1280,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:T44"/>
+  <dimension ref="B1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E3"/>
+      <selection activeCell="X29" sqref="X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1294,48 +1275,49 @@
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="13.75" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="20" width="4" customWidth="1"/>
+    <col min="7" max="14" width="4" hidden="1" customWidth="1"/>
+    <col min="15" max="20" width="4" customWidth="1"/>
     <col min="21" max="21" width="3.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="12" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B2" s="67"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="64" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="64"/>
+      <c r="T2" s="47"/>
     </row>
     <row r="3" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B3" s="50"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
       <c r="G3" s="1">
         <v>1</v>
       </c>
@@ -1379,13 +1361,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B4" s="50" t="s">
+    <row r="4" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B4" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1404,15 +1386,15 @@
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B5" s="50" t="s">
+    <row r="5" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1431,13 +1413,13 @@
       <c r="S5" s="2"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B6" s="50"/>
-      <c r="C6" s="49" t="s">
+    <row r="6" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B6" s="48"/>
+      <c r="C6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1456,15 +1438,15 @@
       <c r="S6" s="2"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B7" s="54" t="s">
+    <row r="7" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B7" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1483,13 +1465,13 @@
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B8" s="55"/>
-      <c r="C8" s="49" t="s">
+    <row r="8" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B8" s="54"/>
+      <c r="C8" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1508,13 +1490,13 @@
       <c r="S8" s="2"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B9" s="55"/>
-      <c r="C9" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+    <row r="9" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B9" s="54"/>
+      <c r="C9" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1533,15 +1515,15 @@
       <c r="S9" s="2"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B10" s="55"/>
-      <c r="C10" s="57" t="s">
+    <row r="10" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B10" s="54"/>
+      <c r="C10" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="21" t="s">
-        <v>43</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="6"/>
@@ -1558,13 +1540,13 @@
       <c r="S10" s="20"/>
       <c r="T10" s="21"/>
     </row>
-    <row r="11" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B11" s="55"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
+    <row r="11" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B11" s="54"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="61"/>
       <c r="F11" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="6"/>
@@ -1581,15 +1563,15 @@
       <c r="S11" s="27"/>
       <c r="T11" s="28"/>
     </row>
-    <row r="12" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B12" s="55"/>
-      <c r="C12" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
+    <row r="12" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B12" s="54"/>
+      <c r="C12" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="57"/>
+      <c r="E12" s="58"/>
       <c r="F12" s="21" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="6"/>
@@ -1606,13 +1588,13 @@
       <c r="S12" s="20"/>
       <c r="T12" s="21"/>
     </row>
-    <row r="13" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B13" s="55"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="62"/>
+    <row r="13" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B13" s="54"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="61"/>
       <c r="F13" s="28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="6"/>
@@ -1629,15 +1611,15 @@
       <c r="S13" s="27"/>
       <c r="T13" s="28"/>
     </row>
-    <row r="14" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B14" s="55"/>
-      <c r="C14" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
+    <row r="14" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B14" s="54"/>
+      <c r="C14" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="57"/>
+      <c r="E14" s="58"/>
       <c r="F14" s="21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="6"/>
@@ -1654,13 +1636,13 @@
       <c r="S14" s="20"/>
       <c r="T14" s="21"/>
     </row>
-    <row r="15" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B15" s="56"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62"/>
+    <row r="15" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B15" s="55"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="61"/>
       <c r="F15" s="28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="6"/>
@@ -1677,15 +1659,15 @@
       <c r="S15" s="27"/>
       <c r="T15" s="28"/>
     </row>
-    <row r="16" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B16" s="50" t="s">
+    <row r="16" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B16" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1704,13 +1686,13 @@
       <c r="S16" s="2"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B17" s="50"/>
-      <c r="C17" s="49" t="s">
+    <row r="17" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B17" s="48"/>
+      <c r="C17" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1730,17 +1712,17 @@
       <c r="T17" s="3"/>
     </row>
     <row r="18" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B18" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="69" t="s">
-        <v>57</v>
+      <c r="B18" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>53</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>23</v>
@@ -1761,11 +1743,11 @@
       <c r="T18" s="23"/>
     </row>
     <row r="19" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B19" s="74"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>23</v>
@@ -1786,11 +1768,11 @@
       <c r="T19" s="23"/>
     </row>
     <row r="20" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B20" s="74"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>23</v>
@@ -1811,11 +1793,11 @@
       <c r="T20" s="23"/>
     </row>
     <row r="21" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B21" s="74"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>23</v>
@@ -1836,14 +1818,14 @@
       <c r="T21" s="23"/>
     </row>
     <row r="22" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B22" s="74"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="71"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
       <c r="E22" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G22" s="24"/>
       <c r="H22" s="31"/>
@@ -1861,13 +1843,13 @@
       <c r="T22" s="32"/>
     </row>
     <row r="23" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B23" s="74"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="69" t="s">
-        <v>52</v>
+      <c r="B23" s="73"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="39" t="s">
+        <v>48</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>24</v>
@@ -1888,11 +1870,11 @@
       <c r="T23" s="23"/>
     </row>
     <row r="24" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B24" s="74"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F24" s="23" t="s">
         <v>24</v>
@@ -1913,14 +1895,14 @@
       <c r="T24" s="23"/>
     </row>
     <row r="25" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B25" s="74"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G25" s="24"/>
       <c r="H25" s="33"/>
@@ -1938,11 +1920,11 @@
       <c r="T25" s="34"/>
     </row>
     <row r="26" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B26" s="74"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
       <c r="E26" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>24</v>
@@ -1963,14 +1945,14 @@
       <c r="T26" s="3"/>
     </row>
     <row r="27" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B27" s="74"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="71"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
       <c r="E27" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="31"/>
@@ -1988,43 +1970,43 @@
       <c r="T27" s="32"/>
     </row>
     <row r="28" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B28" s="74"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="49"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="F28" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="3"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="13"/>
     </row>
     <row r="29" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B29" s="74"/>
-      <c r="C29" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="72" t="s">
-        <v>56</v>
-      </c>
+      <c r="B29" s="73"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="43"/>
       <c r="E29" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>33</v>
+        <v>55</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="12"/>
@@ -2036,147 +2018,145 @@
       <c r="N29" s="11"/>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
       <c r="S29" s="12"/>
       <c r="T29" s="13"/>
     </row>
     <row r="30" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B30" s="74"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="42"/>
+      <c r="F30" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="24"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
       <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="12"/>
-      <c r="T30" s="13"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="23"/>
     </row>
     <row r="31" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B31" s="74"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="53"/>
-      <c r="F31" s="13" t="s">
-        <v>34</v>
+      <c r="B31" s="73"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="42"/>
+      <c r="F31" s="23" t="s">
+        <v>30</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="36"/>
       <c r="M31" s="11"/>
       <c r="N31" s="11"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="22"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
       <c r="R31" s="14"/>
-      <c r="S31" s="12"/>
-      <c r="T31" s="13"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="3"/>
     </row>
     <row r="32" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B32" s="74"/>
-      <c r="C32" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="39" t="s">
-        <v>34</v>
+      <c r="B32" s="73"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="42"/>
+      <c r="F32" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="G32" s="24"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="38"/>
-      <c r="N32" s="38"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
       <c r="O32" s="14"/>
       <c r="P32" s="14"/>
-      <c r="Q32" s="38"/>
-      <c r="R32" s="38"/>
-      <c r="S32" s="38"/>
-      <c r="T32" s="39"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="23"/>
     </row>
     <row r="33" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B33" s="74"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="49"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="42"/>
       <c r="F33" s="23" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G33" s="24"/>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
       <c r="J33" s="22"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="17"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="23"/>
     </row>
     <row r="34" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B34" s="74"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="49"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="42"/>
       <c r="F34" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="G34" s="24"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="23"/>
     </row>
     <row r="35" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B35" s="74"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" s="49"/>
+      <c r="B35" s="73"/>
+      <c r="C35" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="66"/>
+      <c r="E35" s="67"/>
       <c r="F35" s="23" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="G35" s="24"/>
       <c r="H35" s="22"/>
@@ -2184,10 +2164,10 @@
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
       <c r="L35" s="27"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
       <c r="Q35" s="22"/>
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
@@ -2195,238 +2175,162 @@
     </row>
     <row r="36" spans="2:20" ht="17.25" customHeight="1">
       <c r="B36" s="74"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="49" t="s">
+      <c r="C36" s="68"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="23" t="s">
         <v>31</v>
-      </c>
-      <c r="E36" s="49"/>
-      <c r="F36" s="23" t="s">
-        <v>34</v>
       </c>
       <c r="G36" s="24"/>
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
       <c r="J36" s="22"/>
       <c r="K36" s="22"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
       <c r="T36" s="23"/>
     </row>
     <row r="37" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B37" s="74"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="49"/>
+      <c r="B37" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="71"/>
+      <c r="E37" s="45"/>
       <c r="F37" s="23" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G37" s="24"/>
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
       <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
       <c r="S37" s="22"/>
       <c r="T37" s="23"/>
     </row>
-    <row r="38" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B38" s="74"/>
-      <c r="C38" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="44"/>
+    <row r="38" spans="2:20" ht="17.25">
+      <c r="B38" s="48"/>
+      <c r="C38" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="71"/>
       <c r="E38" s="45"/>
       <c r="F38" s="23" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G38" s="24"/>
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
       <c r="S38" s="22"/>
       <c r="T38" s="23"/>
     </row>
-    <row r="39" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B39" s="75"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="48"/>
+    <row r="39" spans="2:20" ht="17.25">
+      <c r="B39" s="48"/>
+      <c r="C39" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="71"/>
+      <c r="E39" s="45"/>
       <c r="F39" s="23" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="G39" s="24"/>
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
       <c r="Q39" s="22"/>
-      <c r="R39" s="22"/>
-      <c r="S39" s="22"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
       <c r="T39" s="23"/>
     </row>
-    <row r="40" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B40" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="52"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="24"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="22"/>
-      <c r="T40" s="23"/>
+    <row r="40" spans="2:20" ht="18" thickBot="1">
+      <c r="B40" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="10"/>
     </row>
     <row r="41" spans="2:20" ht="17.25">
-      <c r="B41" s="50"/>
-      <c r="C41" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="52"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="24"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="22"/>
-      <c r="T41" s="23"/>
-    </row>
-    <row r="42" spans="2:20" ht="17.25">
-      <c r="B42" s="50"/>
-      <c r="C42" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="52"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" s="24"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="23"/>
-    </row>
-    <row r="43" spans="2:20" ht="18" thickBot="1">
-      <c r="B43" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
-      <c r="T43" s="10"/>
-    </row>
-    <row r="44" spans="2:20" ht="17.25">
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="29"/>
+      <c r="S41" s="29"/>
+      <c r="T41" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C18:C28"/>
-    <mergeCell ref="C29:C31"/>
+  <mergeCells count="38">
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="B18:B36"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C6:E6"/>
@@ -2440,20 +2344,18 @@
     <mergeCell ref="C10:E11"/>
     <mergeCell ref="C12:E13"/>
     <mergeCell ref="C14:E15"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="C38:E39"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B18:B39"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C18:C27"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>